<commit_message>
update readme.md & edit the excel file
</commit_message>
<xml_diff>
--- a/Sauce_Demo_Test_Cases_20260107_172452.xlsx
+++ b/Sauce_Demo_Test_Cases_20260107_172452.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portfolio\sample-test-case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E475B-AF88-4366-8F88-9DE812F32DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B438107-0DD7-4A66-8630-BE6C404AA99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -787,17 +787,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -897,10 +898,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -909,22 +910,10 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -935,6 +924,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1256,13 +1257,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1271,10 +1272,10 @@
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -1394,9 +1395,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="A1:H9"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,236 +1411,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="11" t="s">
         <v>221</v>
       </c>
     </row>
@@ -1655,9 +1656,9 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="A1:H12"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1671,314 +1672,314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="11" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2001,272 +2002,272 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="35" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="18"/>
+    <col min="1" max="1" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="35" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="H2" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="H3" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="H4" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="H5" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="H6" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="H7" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="H8" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="H9" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="11" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2298,262 +2299,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="11" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>